<commit_message>
Invert other matrix in Excel
</commit_message>
<xml_diff>
--- a/docs/Matrices.xlsx
+++ b/docs/Matrices.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19416" windowHeight="10728" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19416" windowHeight="10728" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="9" r:id="rId1"/>
@@ -499,10 +499,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.1015625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -510,7 +510,7 @@
     <col min="1" max="16384" width="4.1015625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1">
         <v>3</v>
       </c>
@@ -523,107 +523,68 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="J2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2">
         <v>9</v>
       </c>
       <c r="D3" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F3" s="1">
         <f>SUM(B3:D3)</f>
         <v>15</v>
       </c>
-      <c r="I3" s="2">
-        <v>4</v>
-      </c>
-      <c r="J3" s="2">
-        <v>9</v>
-      </c>
-      <c r="K3" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2">
         <v>3</v>
-      </c>
-      <c r="B4" s="2">
-        <v>7</v>
       </c>
       <c r="C4" s="2">
         <v>5</v>
       </c>
       <c r="D4" s="2">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1">
         <v>3</v>
-      </c>
-      <c r="E4" s="1">
-        <v>7</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" ref="F4:F5" si="0">SUM(B4:D4)</f>
         <v>15</v>
       </c>
-      <c r="H4" s="1">
-        <v>7</v>
-      </c>
-      <c r="I4" s="2">
-        <v>3</v>
-      </c>
-      <c r="J4" s="2">
-        <v>5</v>
-      </c>
-      <c r="K4" s="2">
-        <v>7</v>
-      </c>
-      <c r="L4" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
       </c>
       <c r="D5" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="I5" s="2">
-        <v>8</v>
-      </c>
-      <c r="J5" s="2">
-        <v>1</v>
-      </c>
-      <c r="K5" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" s="1">
         <v>9</v>
       </c>
-      <c r="J6" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="1">
         <f>SUM(B3:B5)</f>
         <v>15</v>
@@ -650,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -679,27 +640,27 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="D3" s="1">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1">
         <v>2</v>
-      </c>
-      <c r="F3" s="1">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C4" s="2">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E4" s="2">
         <v>7</v>
       </c>
       <c r="F4" s="2">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G4" s="2">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="J4" s="1">
         <f>SUM(C4:G4)</f>
@@ -708,25 +669,25 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="1">
+        <v>16</v>
+      </c>
+      <c r="C5" s="2">
         <v>4</v>
       </c>
-      <c r="C5" s="2">
-        <v>16</v>
-      </c>
       <c r="D5" s="2">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E5" s="2">
         <v>25</v>
       </c>
       <c r="F5" s="2">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G5" s="2">
+        <v>16</v>
+      </c>
+      <c r="H5" s="1">
         <v>4</v>
-      </c>
-      <c r="H5" s="1">
-        <v>16</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" ref="J5:J8" si="0">SUM(C5:G5)</f>
@@ -735,25 +696,25 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
+        <v>21</v>
+      </c>
+      <c r="C6" s="2">
+        <v>17</v>
+      </c>
+      <c r="D6" s="2">
         <v>5</v>
-      </c>
-      <c r="C6" s="2">
-        <v>9</v>
-      </c>
-      <c r="D6" s="2">
-        <v>21</v>
       </c>
       <c r="E6" s="2">
         <v>13</v>
       </c>
       <c r="F6" s="2">
+        <v>21</v>
+      </c>
+      <c r="G6" s="2">
+        <v>9</v>
+      </c>
+      <c r="I6" s="1">
         <v>5</v>
-      </c>
-      <c r="G6" s="2">
-        <v>17</v>
-      </c>
-      <c r="I6" s="1">
-        <v>21</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="0"/>
@@ -762,25 +723,25 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="1">
+        <v>22</v>
+      </c>
+      <c r="C7" s="2">
         <v>10</v>
       </c>
-      <c r="C7" s="2">
-        <v>22</v>
-      </c>
       <c r="D7" s="2">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E7" s="2">
         <v>1</v>
       </c>
       <c r="F7" s="2">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G7" s="2">
+        <v>22</v>
+      </c>
+      <c r="H7" s="1">
         <v>10</v>
-      </c>
-      <c r="H7" s="1">
-        <v>22</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="0"/>
@@ -789,19 +750,19 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C8" s="2">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D8" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E8" s="2">
         <v>19</v>
       </c>
       <c r="F8" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G8" s="2">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="0"/>
@@ -810,10 +771,10 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="D9" s="1">
+        <v>24</v>
+      </c>
+      <c r="F9" s="1">
         <v>20</v>
-      </c>
-      <c r="F9" s="1">
-        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">

</xml_diff>